<commit_message>
de volta ao trabalho
</commit_message>
<xml_diff>
--- a/Dados/Checklist QA Fic.xlsx
+++ b/Dados/Checklist QA Fic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98a8b86867ab7286/Área de Trabalho/Dev/Data-Science/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="11_AD4D361C20488DEA4E38A0A4841D54E45ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65594A57-195D-456A-9EC1-F23DAD18F0D3}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="11_AD4D361C20488DEA4E38A0A4841D54E45ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA06EE5B-0774-45E4-B24E-057A154E0A1D}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="37020" yWindow="2535" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -284,6 +284,42 @@
   </si>
   <si>
     <t>Balon Greyjoy</t>
+  </si>
+  <si>
+    <t>Abismo de Helm</t>
+  </si>
+  <si>
+    <t>Acampamento Meio-Sangue</t>
+  </si>
+  <si>
+    <t>Monte Olimpo</t>
+  </si>
+  <si>
+    <t>Submundo</t>
+  </si>
+  <si>
+    <t>Arda - Middle Earth</t>
+  </si>
+  <si>
+    <t>Minas Tirith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theoden </t>
+  </si>
+  <si>
+    <t>Percy Jackson</t>
+  </si>
+  <si>
+    <t>Zeus</t>
+  </si>
+  <si>
+    <t>Hades</t>
+  </si>
+  <si>
+    <t>Eru Illuvatar</t>
+  </si>
+  <si>
+    <t>Gandalf the White</t>
   </si>
 </sst>
 </file>
@@ -667,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,6 +1141,99 @@
         <v>38477</v>
       </c>
     </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="1">
+        <v>29802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="1">
+        <v>27269</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="1">
+        <v>36068</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
tentativa de criar documento excel
</commit_message>
<xml_diff>
--- a/Dados/Checklist QA Fic.xlsx
+++ b/Dados/Checklist QA Fic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98a8b86867ab7286/Área de Trabalho/Dev/Data-Science/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="11_AD4D361C20488DEA4E38A0A4841D54E45ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B973B069-E9A1-456D-915B-055276BF9BDE}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="11_AD4D361C20488DEA4E38A0A4841D54E45ADEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE206887-BC6B-4A4E-87E5-AA40FD70E7D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Resultado Esperado</t>
-  </si>
-  <si>
-    <t>Correto</t>
   </si>
   <si>
     <t>Deveria ter data planejada de início</t>
@@ -793,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,7 +800,7 @@
     <col min="3" max="3" width="13.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="18.21875" customWidth="1"/>
     <col min="10" max="10" width="20.5546875" customWidth="1"/>
@@ -979,7 +976,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1">
         <v>45047</v>
@@ -1428,10 +1425,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
         <v>98</v>
@@ -1454,7 +1451,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
@@ -1477,10 +1474,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
         <v>98</v>
@@ -1503,10 +1500,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
         <v>98</v>
@@ -1529,13 +1526,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
@@ -1555,13 +1552,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
         <v>27</v>
@@ -1581,10 +1578,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
         <v>99</v>
@@ -1604,10 +1601,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
         <v>98</v>
@@ -1630,13 +1627,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
         <v>28</v>
@@ -1656,13 +1653,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" t="s">
         <v>27</v>
@@ -1676,13 +1673,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F31" t="s">
         <v>28</v>
@@ -1696,10 +1693,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
         <v>98</v>

</xml_diff>